<commit_message>
Recommend course api change
</commit_message>
<xml_diff>
--- a/BE/data/Courses Masterdata.xlsx
+++ b/BE/data/Courses Masterdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagarro-my.sharepoint.com/personal/shubham_kargeti_nagarro_com/Documents/Desktop/AI Learning App/BE-MasterBranch/BE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{31936DB6-1694-447D-B4C8-C5DD35CD232D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{105C8857-5D32-48D7-B956-DCB716117EB6}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{31936DB6-1694-447D-B4C8-C5DD35CD232D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5196A32B-F3DD-4226-8418-5B02AE063149}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4386,8 +4386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21011,7 +21011,7 @@
       <c r="G573" s="1" t="s">
         <v>1329</v>
       </c>
-      <c r="H573" s="1" t="s">
+      <c r="H573" s="2" t="s">
         <v>680</v>
       </c>
       <c r="I573" t="s">
@@ -21044,6 +21044,7 @@
     <hyperlink ref="H23" r:id="rId22" xr:uid="{6872C5E7-F542-4596-8360-5C1C15DA7087}"/>
     <hyperlink ref="H24" r:id="rId23" xr:uid="{23C4D713-DDC6-4D60-ADA0-A7EFAE14E106}"/>
     <hyperlink ref="H25" r:id="rId24" xr:uid="{8C393239-12C9-4FA0-A228-E5E5B3FA7E69}"/>
+    <hyperlink ref="H573" r:id="rId25" xr:uid="{C711438C-D580-4A4E-8582-2AEFD51DE57A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>